<commit_message>
template updates; master script divide by zero error fix
</commit_message>
<xml_diff>
--- a/PPA2/Input_Template/XLSX/PPA_Template_ArterialExp.xlsx
+++ b/PPA2/Input_Template/XLSX/PPA_Template_ArterialExp.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Q:\ProjectLevelPerformanceAssessment\PPAv2\PPA2_0_code\PPA2\Input_Template\XLSX\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD329062-6B67-4176-ABEE-E1D18154FAAB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02B231A5-6BCE-480D-911A-E0313C15B475}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13096" tabRatio="712" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13665" yWindow="735" windowWidth="15165" windowHeight="14970" tabRatio="712" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="0ATitlePg" sheetId="4" r:id="rId1"/>
@@ -26,13 +26,17 @@
     <sheet name="import" sheetId="1" r:id="rId11"/>
     <sheet name="lookup_helper" sheetId="5" r:id="rId12"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId13"/>
+    <externalReference r:id="rId14"/>
+  </externalReferences>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="10" hidden="1">import!$A$1:$G$117</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="11" hidden="1">lookup_helper!$A$3:$I$119</definedName>
     <definedName name="_Hlk20929805" localSheetId="5">'4EconProsperity'!$A$68</definedName>
     <definedName name="_Hlk20929868" localSheetId="8">'7SGR'!$A$4</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="2">'1ReduceVMT'!$A$1:$H$68</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="4">'3Multimodal'!$A$1:$H$78</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="4">'3Multimodal'!$A$1:$H$115</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="6">'5Freight'!$A$1:$H$66</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="9">'8SocioEconEquity'!$A$1:$H$88</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="2">'1ReduceVMT'!$1:$2</definedName>
@@ -59,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="643" uniqueCount="310">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="647" uniqueCount="314">
   <si>
     <t>data_item</t>
   </si>
@@ -1032,6 +1036,18 @@
   </si>
   <si>
     <t>On project segment*</t>
+  </si>
+  <si>
+    <t>Multi-modal indicator 4: Residential Mode Split:</t>
+  </si>
+  <si>
+    <t>NOTE - The 2040 mode split shown below is based on modeled values estimated</t>
+  </si>
+  <si>
+    <t>for SACOG's 2020 MTP-SCS. As with all other 2040 values in this report, they do NOT factor in</t>
+  </si>
+  <si>
+    <t>the potential effects of the project for which this report was generated.</t>
   </si>
 </sst>
 </file>
@@ -2585,6 +2601,355 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.12411111111111112"/>
+          <c:y val="3.8567493112947659E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>lookup_helper!$B$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Share of land that is Ag use within project area</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:numRef>
+              <c:f>lookup_helper!$D$3:$E$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>2016</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2040</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>lookup_helper!$D$5:$E$5</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0.1236248623319337</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-8390-4D02-8EE7-F8C606E9DD59}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1814706704"/>
+        <c:axId val="1818653760"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1814706704"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1818653760"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1818653760"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0%" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1814706704"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup orientation="landscape"/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
       <c:tx>
         <c:rich>
           <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
@@ -2925,7 +3290,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -3552,7 +3917,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -3973,7 +4338,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart14.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -4408,7 +4773,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart15.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -4843,7 +5208,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart16.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -8465,6 +8830,386 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Residential Mode Split within 0.5mi of Project</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Location</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </c:spPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>lookup_helper!$D$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>2016</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>lookup_helper!$B$7:$B$11</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Single-occupant vehicle trips</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Carpool trips</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Transit trips</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Biking trips</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Walking trips</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>lookup_helper!$D$7:$D$11</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.34736895830143422</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.5294237737967642</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9.3911090695656604E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.9445720410350639E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.7884958913897823E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-C62D-49B8-9613-A3A302B5F080}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>lookup_helper!$E$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>2040</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>lookup_helper!$E$7:$E$11</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.36404675917126023</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.49786162326553879</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.397072799847938E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.0385858201862759E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8.6818095419121846E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-C62D-49B8-9613-A3A302B5F080}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="55"/>
+        <c:axId val="1126743616"/>
+        <c:axId val="1440870240"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1126743616"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:prstDash val="solid"/>
+            <a:round/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1440870240"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1440870240"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:prstDash val="solid"/>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0%" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+            <a:prstDash val="solid"/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1126743616"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
               <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
@@ -9199,7 +9944,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -9939,355 +10684,6 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:layout>
-        <c:manualLayout>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="0.12411111111111112"/>
-          <c:y val="3.8567493112947659E-2"/>
-        </c:manualLayout>
-      </c:layout>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>lookup_helper!$B$5</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Share of land that is Ag use within project area</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:dLbls>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="75000"/>
-                        <a:lumOff val="25000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="en-US"/>
-              </a:p>
-            </c:txPr>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:showLeaderLines val="1"/>
-                <c15:leaderLines>
-                  <c:spPr>
-                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="35000"/>
-                          <a:lumOff val="65000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:round/>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c15:leaderLines>
-              </c:ext>
-            </c:extLst>
-          </c:dLbls>
-          <c:cat>
-            <c:numRef>
-              <c:f>lookup_helper!$D$3:$E$3</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>2016</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2040</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>lookup_helper!$D$5:$E$5</c:f>
-              <c:numCache>
-                <c:formatCode>0%</c:formatCode>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>0.1236248623319337</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-8390-4D02-8EE7-F8C606E9DD59}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="219"/>
-        <c:overlap val="-27"/>
-        <c:axId val="1814706704"/>
-        <c:axId val="1818653760"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="1814706704"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="1818653760"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="1818653760"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-          <c:min val="0"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="0%" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="1814706704"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup orientation="landscape"/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -18672,6 +19068,49 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>99</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>114</xdr:row>
+      <xdr:rowOff>82550</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{20D56D8E-7A9C-4950-9976-B43B284F06B9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
       <xdr:colOff>61911</xdr:colOff>
       <xdr:row>11</xdr:row>
       <xdr:rowOff>57149</xdr:rowOff>
@@ -18784,7 +19223,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -18825,7 +19264,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -18866,7 +19305,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -18985,7 +19424,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -19026,6 +19465,156 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="0ATitlePg"/>
+      <sheetName val="0BUsingThisReport"/>
+      <sheetName val="3Multimodal"/>
+      <sheetName val="4EconProsperity"/>
+      <sheetName val="6Safety"/>
+      <sheetName val="8SocioEconEquity"/>
+      <sheetName val="1ReduceVMT"/>
+      <sheetName val="2ReduceCongestion"/>
+      <sheetName val="5Freight"/>
+      <sheetName val="7SGR"/>
+      <sheetName val="import"/>
+      <sheetName val="lookup_helper"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="3" refreshError="1"/>
+      <sheetData sheetId="4" refreshError="1"/>
+      <sheetData sheetId="5" refreshError="1"/>
+      <sheetData sheetId="6" refreshError="1"/>
+      <sheetData sheetId="7" refreshError="1"/>
+      <sheetData sheetId="8" refreshError="1"/>
+      <sheetData sheetId="9" refreshError="1"/>
+      <sheetData sheetId="10" refreshError="1"/>
+      <sheetData sheetId="11">
+        <row r="3">
+          <cell r="D3">
+            <v>2016</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="B7" t="str">
+            <v>Single-occupant vehicle trips</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="B8" t="str">
+            <v>Carpool trips</v>
+          </cell>
+        </row>
+        <row r="9">
+          <cell r="B9" t="str">
+            <v>Transit trips</v>
+          </cell>
+        </row>
+        <row r="10">
+          <cell r="B10" t="str">
+            <v>Biking trips</v>
+          </cell>
+        </row>
+        <row r="11">
+          <cell r="B11" t="str">
+            <v>Walking trips</v>
+          </cell>
+        </row>
+      </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="0ATitlePg"/>
+      <sheetName val="0BUsingThisReport"/>
+      <sheetName val="1ReduceVMT"/>
+      <sheetName val="2ReduceCongestion"/>
+      <sheetName val="3Multimodal"/>
+      <sheetName val="4EconProsperity"/>
+      <sheetName val="5Freight"/>
+      <sheetName val="6Safety"/>
+      <sheetName val="7SGR"/>
+      <sheetName val="8SocioEconEquity"/>
+      <sheetName val="import"/>
+      <sheetName val="lookup_helper"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
+      <sheetData sheetId="7"/>
+      <sheetData sheetId="8"/>
+      <sheetData sheetId="9"/>
+      <sheetData sheetId="10"/>
+      <sheetData sheetId="11">
+        <row r="3">
+          <cell r="D3">
+            <v>2016</v>
+          </cell>
+          <cell r="E3">
+            <v>2040</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="D7">
+            <v>0.34736895830143422</v>
+          </cell>
+          <cell r="E7">
+            <v>0.36404675917126023</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="D8">
+            <v>0.5294237737967642</v>
+          </cell>
+          <cell r="E8">
+            <v>0.49786162326553879</v>
+          </cell>
+        </row>
+        <row r="9">
+          <cell r="D9">
+            <v>9.3911090695656604E-3</v>
+          </cell>
+          <cell r="E9">
+            <v>1.397072799847938E-2</v>
+          </cell>
+        </row>
+        <row r="10">
+          <cell r="D10">
+            <v>1.9445720410350639E-2</v>
+          </cell>
+          <cell r="E10">
+            <v>2.0385858201862759E-2</v>
+          </cell>
+        </row>
+        <row r="11">
+          <cell r="D11">
+            <v>7.7884958913897823E-2</v>
+          </cell>
+          <cell r="E11">
+            <v>8.6818095419121846E-2</v>
+          </cell>
+        </row>
+      </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -20969,8 +21558,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:R119"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A68" activePane="bottomLeft" state="frozen"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="K90" sqref="K90"/>
       <selection pane="bottomLeft" activeCell="K90" sqref="K90"/>
     </sheetView>
@@ -25934,11 +26523,9 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87207DCC-1888-4FF1-B645-7715A9482FCA}">
   <sheetPr codeName="Sheet6"/>
-  <dimension ref="A1:I56"/>
+  <dimension ref="A1:I98"/>
   <sheetViews>
-    <sheetView showWhiteSpace="0" view="pageLayout" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
-    </sheetView>
+    <sheetView view="pageLayout" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -25946,6 +26533,7 @@
     <col min="2" max="2" width="17.5703125" customWidth="1"/>
     <col min="3" max="3" width="15.28515625" customWidth="1"/>
     <col min="4" max="5" width="5.42578125" customWidth="1"/>
+    <col min="8" max="8" width="14.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="65" customFormat="1" x14ac:dyDescent="0.25">
@@ -26120,6 +26708,26 @@
         <v>229</v>
       </c>
     </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A95" s="29" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A96" s="46" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A97" s="46" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A98" s="46" t="s">
+        <v>313</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A12:E12"/>
@@ -26127,10 +26735,12 @@
     <mergeCell ref="A14:C14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-  <rowBreaks count="1" manualBreakCount="1">
+  <pageSetup scale="90" orientation="portrait" r:id="rId1"/>
+  <rowBreaks count="2" manualBreakCount="2">
     <brk id="42" max="7" man="1"/>
+    <brk id="91" max="7" man="1"/>
   </rowBreaks>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
fix minor bugs in arterial exp and CS XLSX templates
</commit_message>
<xml_diff>
--- a/PPA2/Input_Template/XLSX/PPA_Template_ArterialExp.xlsx
+++ b/PPA2/Input_Template/XLSX/PPA_Template_ArterialExp.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Q:\ProjectLevelPerformanceAssessment\PPAv2\PPA2_0_code\PPA2\Input_Template\XLSX\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02B231A5-6BCE-480D-911A-E0313C15B475}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{808729FF-1413-45C0-8BB8-02B4EEB7514A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13665" yWindow="735" windowWidth="15165" windowHeight="14970" tabRatio="712" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="712" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="0ATitlePg" sheetId="4" r:id="rId1"/>
@@ -26,10 +26,6 @@
     <sheet name="import" sheetId="1" r:id="rId11"/>
     <sheet name="lookup_helper" sheetId="5" r:id="rId12"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId13"/>
-    <externalReference r:id="rId14"/>
-  </externalReferences>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="10" hidden="1">import!$A$1:$G$117</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="11" hidden="1">lookup_helper!$A$3:$I$119</definedName>
@@ -988,9 +984,6 @@
     <t>Economic Prosperity Indicator 5: Change in Ag acreage share within 0.5mi of project location</t>
   </si>
   <si>
-    <t>Safety Indicator 4: Bike + Ped Fatalities per Project Centerline Mile</t>
-  </si>
-  <si>
     <t>Bike/ped collisions per road centerline mile</t>
   </si>
   <si>
@@ -1048,6 +1041,9 @@
   </si>
   <si>
     <t>the potential effects of the project for which this report was generated.</t>
+  </si>
+  <si>
+    <t>Safety Indicator 4: Bike + Ped Collisions per Project Centerline Mile</t>
   </si>
 </sst>
 </file>
@@ -19467,156 +19463,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="0ATitlePg"/>
-      <sheetName val="0BUsingThisReport"/>
-      <sheetName val="3Multimodal"/>
-      <sheetName val="4EconProsperity"/>
-      <sheetName val="6Safety"/>
-      <sheetName val="8SocioEconEquity"/>
-      <sheetName val="1ReduceVMT"/>
-      <sheetName val="2ReduceCongestion"/>
-      <sheetName val="5Freight"/>
-      <sheetName val="7SGR"/>
-      <sheetName val="import"/>
-      <sheetName val="lookup_helper"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-      <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2" refreshError="1"/>
-      <sheetData sheetId="3" refreshError="1"/>
-      <sheetData sheetId="4" refreshError="1"/>
-      <sheetData sheetId="5" refreshError="1"/>
-      <sheetData sheetId="6" refreshError="1"/>
-      <sheetData sheetId="7" refreshError="1"/>
-      <sheetData sheetId="8" refreshError="1"/>
-      <sheetData sheetId="9" refreshError="1"/>
-      <sheetData sheetId="10" refreshError="1"/>
-      <sheetData sheetId="11">
-        <row r="3">
-          <cell r="D3">
-            <v>2016</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="B7" t="str">
-            <v>Single-occupant vehicle trips</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="B8" t="str">
-            <v>Carpool trips</v>
-          </cell>
-        </row>
-        <row r="9">
-          <cell r="B9" t="str">
-            <v>Transit trips</v>
-          </cell>
-        </row>
-        <row r="10">
-          <cell r="B10" t="str">
-            <v>Biking trips</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="B11" t="str">
-            <v>Walking trips</v>
-          </cell>
-        </row>
-      </sheetData>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="0ATitlePg"/>
-      <sheetName val="0BUsingThisReport"/>
-      <sheetName val="1ReduceVMT"/>
-      <sheetName val="2ReduceCongestion"/>
-      <sheetName val="3Multimodal"/>
-      <sheetName val="4EconProsperity"/>
-      <sheetName val="5Freight"/>
-      <sheetName val="6Safety"/>
-      <sheetName val="7SGR"/>
-      <sheetName val="8SocioEconEquity"/>
-      <sheetName val="import"/>
-      <sheetName val="lookup_helper"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
-      <sheetData sheetId="7"/>
-      <sheetData sheetId="8"/>
-      <sheetData sheetId="9"/>
-      <sheetData sheetId="10"/>
-      <sheetData sheetId="11">
-        <row r="3">
-          <cell r="D3">
-            <v>2016</v>
-          </cell>
-          <cell r="E3">
-            <v>2040</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="D7">
-            <v>0.34736895830143422</v>
-          </cell>
-          <cell r="E7">
-            <v>0.36404675917126023</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="D8">
-            <v>0.5294237737967642</v>
-          </cell>
-          <cell r="E8">
-            <v>0.49786162326553879</v>
-          </cell>
-        </row>
-        <row r="9">
-          <cell r="D9">
-            <v>9.3911090695656604E-3</v>
-          </cell>
-          <cell r="E9">
-            <v>1.397072799847938E-2</v>
-          </cell>
-        </row>
-        <row r="10">
-          <cell r="D10">
-            <v>1.9445720410350639E-2</v>
-          </cell>
-          <cell r="E10">
-            <v>2.0385858201862759E-2</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="D11">
-            <v>7.7884958913897823E-2</v>
-          </cell>
-          <cell r="E11">
-            <v>8.6818095419121846E-2</v>
-          </cell>
-        </row>
-      </sheetData>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -20123,7 +19969,7 @@
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="55" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B43" s="11"/>
       <c r="C43" s="11"/>
@@ -21561,7 +21407,7 @@
     <sheetView topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="K90" sqref="K90"/>
-      <selection pane="bottomLeft" activeCell="K90" sqref="K90"/>
+      <selection pane="bottomLeft" activeCell="G1" sqref="G1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -24929,7 +24775,7 @@
         <v>25</v>
       </c>
       <c r="B92" s="28" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C92" t="s">
         <v>205</v>
@@ -26015,7 +25861,7 @@
     </row>
     <row r="6" spans="1:9" ht="159" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="94" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B6" s="94"/>
       <c r="C6" s="94"/>
@@ -26033,7 +25879,7 @@
     </row>
     <row r="10" spans="1:9" ht="223.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="94" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B10" s="94"/>
       <c r="C10" s="94"/>
@@ -26710,22 +26556,22 @@
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A95" s="29" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A96" s="46" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A97" s="46" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A98" s="46" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
   </sheetData>
@@ -27059,8 +26905,8 @@
   <sheetPr codeName="Sheet9"/>
   <dimension ref="A1:H72"/>
   <sheetViews>
-    <sheetView view="pageLayout" topLeftCell="A52" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A70" sqref="A70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -27124,7 +26970,7 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="29" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -27137,7 +26983,7 @@
     </row>
     <row r="37" spans="1:3" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="34" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B37" s="35" t="s">
         <v>234</v>
@@ -27162,7 +27008,7 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
@@ -27172,12 +27018,12 @@
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" s="29" t="s">
-        <v>302</v>
+        <v>313</v>
       </c>
     </row>
     <row r="70" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A70" s="83" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="71" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>